<commit_message>
upd master 19 Feb
</commit_message>
<xml_diff>
--- a/Customer/Cust 2025/Cargo DX 2025.xlsx
+++ b/Customer/Cust 2025/Cargo DX 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick Jonathan\Documents\Patrick Jonathan\CARGO\Cargo Work\Customer\Cust 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCBC1816-6324-4D10-A375-A00D5D602471}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1A03D2-54E0-4A61-8FBF-9ED4803523A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E000C531-AA46-4CF4-8BD7-2185A135A010}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E000C531-AA46-4CF4-8BD7-2185A135A010}"/>
   </bookViews>
   <sheets>
     <sheet name="SEA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
   <si>
     <t>Hijau barang terkirim, Lunas, beres</t>
   </si>
@@ -236,6 +236,99 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>A0034794</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Comic Sans MS"/>
+        <charset val="134"/>
+      </rPr>
+      <t>LHT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>联昊通：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Comic Sans MS"/>
+        <charset val="134"/>
+      </rPr>
+      <t>901446273786</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Comic Sans MS"/>
+        <charset val="134"/>
+      </rPr>
+      <t>LED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>灯</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Comic Sans MS"/>
+        <charset val="134"/>
+      </rPr>
+      <t>LED lamp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>运费52</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Comic Sans MS"/>
+        <charset val="134"/>
+      </rPr>
+      <t>RMB</t>
+    </r>
+  </si>
+  <si>
+    <t>A20</t>
+  </si>
+  <si>
+    <t>A21</t>
+  </si>
+  <si>
+    <t>A22</t>
   </si>
 </sst>
 </file>
@@ -335,7 +428,7 @@
       <family val="4"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -393,6 +486,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFB0BCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -467,7 +566,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -580,33 +679,66 @@
     <xf numFmtId="0" fontId="11" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="8" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="170" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="167" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="169" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -616,37 +748,49 @@
     <xf numFmtId="169" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="8" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="170" fontId="10" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -967,7 +1111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03568550-BD00-482C-9F46-E2F5DB6F38F1}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
@@ -1049,11 +1193,11 @@
       <c r="J2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
       <c r="N2" s="18" t="s">
         <v>16</v>
       </c>
@@ -1065,10 +1209,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="33.75">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="39"/>
+      <c r="B3" s="47"/>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
       <c r="E3" s="22"/>
@@ -1088,7 +1232,7 @@
       <c r="B5" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C5" s="52" t="s">
+      <c r="C5" s="38" t="s">
         <v>34</v>
       </c>
       <c r="D5" s="28" t="s">
@@ -1097,7 +1241,7 @@
       <c r="E5" s="29">
         <v>45702</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="39" t="s">
         <v>36</v>
       </c>
       <c r="G5" s="30" t="s">
@@ -1109,7 +1253,7 @@
       <c r="I5" s="28">
         <v>22</v>
       </c>
-      <c r="J5" s="54">
+      <c r="J5" s="40">
         <v>0.11761200000000001</v>
       </c>
       <c r="K5" s="28">
@@ -1130,29 +1274,29 @@
       <c r="P5" s="28"/>
     </row>
     <row r="6" spans="1:16" ht="22.5">
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="56" t="s">
+      <c r="C6" s="48"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="48"/>
+      <c r="F6" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="57"/>
-      <c r="H6" s="58"/>
-      <c r="I6" s="58">
+      <c r="G6" s="42"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43">
         <v>22</v>
       </c>
-      <c r="J6" s="59">
+      <c r="J6" s="44">
         <v>0.11761200000000001</v>
       </c>
-      <c r="K6" s="58"/>
-      <c r="L6" s="58"/>
-      <c r="M6" s="58"/>
-      <c r="N6" s="60"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="60"/>
+      <c r="K6" s="43"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="43"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="45"/>
+      <c r="P6" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1166,9 +1310,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DD94FD-D993-429D-A766-D707FAC76EEB}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
@@ -1250,11 +1394,11 @@
       <c r="J2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
       <c r="N2" s="18" t="s">
         <v>16</v>
       </c>
@@ -1266,10 +1410,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="33.75">
-      <c r="A3" s="40" t="s">
+      <c r="A3" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="40"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
       <c r="E3" s="22"/>
@@ -1295,7 +1439,7 @@
       <c r="C5" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="52" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="29">
@@ -1304,32 +1448,32 @@
       <c r="F5" s="28">
         <v>1</v>
       </c>
-      <c r="G5" s="44" t="s">
+      <c r="G5" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="41">
+      <c r="H5" s="52">
         <v>62</v>
       </c>
-      <c r="I5" s="41">
+      <c r="I5" s="52">
         <v>11.7</v>
       </c>
-      <c r="J5" s="47">
+      <c r="J5" s="58">
         <f>K5*L5*M5/1000000</f>
         <v>4.8543999999999997E-2</v>
       </c>
-      <c r="K5" s="41">
+      <c r="K5" s="52">
         <v>32</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="52">
         <v>37</v>
       </c>
-      <c r="M5" s="41">
+      <c r="M5" s="52">
         <v>41</v>
       </c>
       <c r="N5" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="44" t="s">
+      <c r="O5" s="49" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1337,51 +1481,51 @@
       <c r="A6" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="50">
+      <c r="D6" s="57"/>
+      <c r="E6" s="54">
         <v>45673</v>
       </c>
       <c r="F6" s="28">
         <v>1</v>
       </c>
-      <c r="G6" s="45"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="44" t="s">
+      <c r="G6" s="50"/>
+      <c r="H6" s="57"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="45"/>
+      <c r="O6" s="50"/>
     </row>
     <row r="7" spans="1:16" ht="21">
       <c r="A7" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43"/>
-      <c r="E7" s="51"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="55"/>
       <c r="F7" s="28">
         <v>2</v>
       </c>
-      <c r="G7" s="46"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="49"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-      <c r="M7" s="43"/>
-      <c r="N7" s="46"/>
-      <c r="O7" s="46"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="60"/>
+      <c r="K7" s="53"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="51"/>
+      <c r="O7" s="51"/>
     </row>
     <row r="8" spans="1:16" ht="22.5">
       <c r="A8" s="31"/>
@@ -1408,13 +1552,176 @@
       <c r="N8" s="37"/>
       <c r="O8" s="37"/>
     </row>
+    <row r="9" spans="1:16" ht="21">
+      <c r="A9" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="63">
+        <v>45706</v>
+      </c>
+      <c r="F9" s="61">
+        <v>1</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" s="62">
+        <v>16</v>
+      </c>
+      <c r="I9" s="61">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J9" s="64">
+        <v>3.7975000000000002E-2</v>
+      </c>
+      <c r="K9" s="61">
+        <v>49</v>
+      </c>
+      <c r="L9" s="61">
+        <v>25</v>
+      </c>
+      <c r="M9" s="61">
+        <v>31</v>
+      </c>
+      <c r="N9" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="O9" s="61"/>
+    </row>
+    <row r="10" spans="1:16" ht="21">
+      <c r="A10" s="61" t="s">
+        <v>46</v>
+      </c>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="61">
+        <v>2</v>
+      </c>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="61">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J10" s="64">
+        <v>3.7975000000000002E-2</v>
+      </c>
+      <c r="K10" s="61">
+        <v>49</v>
+      </c>
+      <c r="L10" s="61">
+        <v>25</v>
+      </c>
+      <c r="M10" s="61">
+        <v>31</v>
+      </c>
+      <c r="N10" s="68"/>
+      <c r="O10" s="61"/>
+    </row>
+    <row r="11" spans="1:16" ht="21">
+      <c r="A11" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="67"/>
+      <c r="F11" s="61">
+        <v>3</v>
+      </c>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="61">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J11" s="64">
+        <v>3.7975000000000002E-2</v>
+      </c>
+      <c r="K11" s="61">
+        <v>49</v>
+      </c>
+      <c r="L11" s="61">
+        <v>25</v>
+      </c>
+      <c r="M11" s="61">
+        <v>31</v>
+      </c>
+      <c r="N11" s="68"/>
+      <c r="O11" s="61"/>
+    </row>
+    <row r="12" spans="1:16" ht="21">
+      <c r="A12" s="61" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="70"/>
+      <c r="F12" s="61">
+        <v>4</v>
+      </c>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="61">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J12" s="64">
+        <v>3.7975000000000002E-2</v>
+      </c>
+      <c r="K12" s="61">
+        <v>49</v>
+      </c>
+      <c r="L12" s="61">
+        <v>25</v>
+      </c>
+      <c r="M12" s="61">
+        <v>31</v>
+      </c>
+      <c r="N12" s="71"/>
+      <c r="O12" s="61"/>
+    </row>
+    <row r="13" spans="1:16" ht="22.5">
+      <c r="A13" s="72"/>
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="33">
+        <v>4</v>
+      </c>
+      <c r="G13" s="35"/>
+      <c r="H13" s="35"/>
+      <c r="I13" s="33">
+        <v>40.799999999999997</v>
+      </c>
+      <c r="J13" s="73">
+        <v>0.15190000000000001</v>
+      </c>
+      <c r="K13" s="33"/>
+      <c r="L13" s="33"/>
+      <c r="M13" s="33"/>
+      <c r="N13" s="74"/>
+      <c r="O13" s="75"/>
+    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="N6:N7"/>
+  <mergeCells count="22">
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="G9:G12"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D5:D7"/>
@@ -1425,6 +1732,11 @@
     <mergeCell ref="K5:K7"/>
     <mergeCell ref="L5:L7"/>
     <mergeCell ref="M5:M7"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="N6:N7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
upd master 26 Feb
</commit_message>
<xml_diff>
--- a/Customer/Cust 2025/Cargo DX 2025.xlsx
+++ b/Customer/Cust 2025/Cargo DX 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick Jonathan\Documents\Patrick Jonathan\CARGO\Cargo Work\Customer\Cust 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1A03D2-54E0-4A61-8FBF-9ED4803523A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1862FCBC-522F-480A-BB07-D382D2D4AE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{E000C531-AA46-4CF4-8BD7-2185A135A010}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E000C531-AA46-4CF4-8BD7-2185A135A010}"/>
   </bookViews>
   <sheets>
     <sheet name="SEA" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="49">
   <si>
     <t>Hijau barang terkirim, Lunas, beres</t>
   </si>
@@ -229,9 +229,6 @@
     <t>智能家居Smart home</t>
   </si>
   <si>
-    <t>退税TR</t>
-  </si>
-  <si>
     <t>TOTAL</t>
   </si>
   <si>
@@ -329,6 +326,10 @@
   </si>
   <si>
     <t>A22</t>
+  </si>
+  <si>
+    <t>F1286
+退税TR</t>
   </si>
 </sst>
 </file>
@@ -566,7 +567,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -703,6 +704,24 @@
     <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="8" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -712,33 +731,54 @@
     <xf numFmtId="0" fontId="12" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="169" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -748,49 +788,13 @@
     <xf numFmtId="169" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="8" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1111,7 +1115,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03568550-BD00-482C-9F46-E2F5DB6F38F1}">
   <dimension ref="A1:P6"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
@@ -1193,11 +1197,11 @@
       <c r="J2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
       <c r="N2" s="18" t="s">
         <v>16</v>
       </c>
@@ -1209,10 +1213,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="33.75">
-      <c r="A3" s="47" t="s">
+      <c r="A3" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="47"/>
+      <c r="B3" s="53"/>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
       <c r="E3" s="22"/>
@@ -1228,7 +1232,7 @@
       <c r="O3" s="24"/>
       <c r="P3" s="25"/>
     </row>
-    <row r="5" spans="1:16" ht="21">
+    <row r="5" spans="1:16" ht="42">
       <c r="B5" s="28" t="s">
         <v>33</v>
       </c>
@@ -1265,23 +1269,25 @@
       <c r="M5" s="28">
         <v>27</v>
       </c>
-      <c r="N5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="O5" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="P5" s="28"/>
+      <c r="N5" s="76">
+        <v>45706</v>
+      </c>
+      <c r="O5" s="76">
+        <v>45735</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="6" spans="1:16" ht="22.5">
-      <c r="B6" s="48" t="s">
+      <c r="B6" s="54" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="54"/>
+      <c r="D6" s="54"/>
+      <c r="E6" s="54"/>
+      <c r="F6" s="41" t="s">
         <v>39</v>
-      </c>
-      <c r="C6" s="48"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="48"/>
-      <c r="F6" s="41" t="s">
-        <v>40</v>
       </c>
       <c r="G6" s="42"/>
       <c r="H6" s="43"/>
@@ -1312,7 +1318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DD94FD-D993-429D-A766-D707FAC76EEB}">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
@@ -1394,11 +1400,11 @@
       <c r="J2" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="46" t="s">
+      <c r="K2" s="52" t="s">
         <v>15</v>
       </c>
-      <c r="L2" s="46"/>
-      <c r="M2" s="46"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="52"/>
       <c r="N2" s="18" t="s">
         <v>16</v>
       </c>
@@ -1410,10 +1416,10 @@
       </c>
     </row>
     <row r="3" spans="1:16" ht="33.75">
-      <c r="A3" s="56" t="s">
+      <c r="A3" s="64" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="56"/>
+      <c r="B3" s="64"/>
       <c r="C3" s="20"/>
       <c r="D3" s="21"/>
       <c r="E3" s="22"/>
@@ -1439,7 +1445,7 @@
       <c r="C5" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="52" t="s">
+      <c r="D5" s="65" t="s">
         <v>24</v>
       </c>
       <c r="E5" s="29">
@@ -1448,32 +1454,32 @@
       <c r="F5" s="28">
         <v>1</v>
       </c>
-      <c r="G5" s="49" t="s">
+      <c r="G5" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="52">
+      <c r="H5" s="65">
         <v>62</v>
       </c>
-      <c r="I5" s="52">
+      <c r="I5" s="65">
         <v>11.7</v>
       </c>
-      <c r="J5" s="58">
+      <c r="J5" s="71">
         <f>K5*L5*M5/1000000</f>
         <v>4.8543999999999997E-2</v>
       </c>
-      <c r="K5" s="52">
+      <c r="K5" s="65">
         <v>32</v>
       </c>
-      <c r="L5" s="52">
+      <c r="L5" s="65">
         <v>37</v>
       </c>
-      <c r="M5" s="52">
+      <c r="M5" s="65">
         <v>41</v>
       </c>
       <c r="N5" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="O5" s="49" t="s">
+      <c r="O5" s="68" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1481,51 +1487,51 @@
       <c r="A6" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="52" t="s">
+      <c r="B6" s="65" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="54">
+      <c r="D6" s="66"/>
+      <c r="E6" s="74">
         <v>45673</v>
       </c>
       <c r="F6" s="28">
         <v>1</v>
       </c>
-      <c r="G6" s="50"/>
-      <c r="H6" s="57"/>
-      <c r="I6" s="57"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="49" t="s">
+      <c r="G6" s="69"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="66"/>
+      <c r="J6" s="72"/>
+      <c r="K6" s="66"/>
+      <c r="L6" s="66"/>
+      <c r="M6" s="66"/>
+      <c r="N6" s="68" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="50"/>
+      <c r="O6" s="69"/>
     </row>
     <row r="7" spans="1:16" ht="21">
       <c r="A7" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="55"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="75"/>
       <c r="F7" s="28">
         <v>2</v>
       </c>
-      <c r="G7" s="51"/>
-      <c r="H7" s="53"/>
-      <c r="I7" s="53"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="53"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="53"/>
-      <c r="N7" s="51"/>
-      <c r="O7" s="51"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="67"/>
+      <c r="L7" s="67"/>
+      <c r="M7" s="67"/>
+      <c r="N7" s="70"/>
+      <c r="O7" s="70"/>
     </row>
     <row r="8" spans="1:16" ht="22.5">
       <c r="A8" s="31"/>
@@ -1553,149 +1559,149 @@
       <c r="O8" s="37"/>
     </row>
     <row r="9" spans="1:16" ht="21">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="46" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="B9" s="62" t="s">
+      <c r="C9" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="62" t="s">
+      <c r="D9" s="55" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="61">
+        <v>45706</v>
+      </c>
+      <c r="F9" s="46">
+        <v>1</v>
+      </c>
+      <c r="G9" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="D9" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="63">
-        <v>45706</v>
-      </c>
-      <c r="F9" s="61">
-        <v>1</v>
-      </c>
-      <c r="G9" s="62" t="s">
+      <c r="H9" s="55">
+        <v>16</v>
+      </c>
+      <c r="I9" s="46">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="J9" s="47">
+        <v>3.7975000000000002E-2</v>
+      </c>
+      <c r="K9" s="46">
+        <v>49</v>
+      </c>
+      <c r="L9" s="46">
+        <v>25</v>
+      </c>
+      <c r="M9" s="46">
+        <v>31</v>
+      </c>
+      <c r="N9" s="58" t="s">
         <v>44</v>
       </c>
-      <c r="H9" s="62">
-        <v>16</v>
-      </c>
-      <c r="I9" s="61">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="J9" s="64">
-        <v>3.7975000000000002E-2</v>
-      </c>
-      <c r="K9" s="61">
-        <v>49</v>
-      </c>
-      <c r="L9" s="61">
-        <v>25</v>
-      </c>
-      <c r="M9" s="61">
-        <v>31</v>
-      </c>
-      <c r="N9" s="65" t="s">
-        <v>45</v>
-      </c>
-      <c r="O9" s="61"/>
+      <c r="O9" s="46"/>
     </row>
     <row r="10" spans="1:16" ht="21">
-      <c r="A10" s="61" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="61">
+      <c r="A10" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="56"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="56"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="46">
         <v>2</v>
       </c>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="61">
+      <c r="G10" s="56"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="46">
         <v>10.199999999999999</v>
       </c>
-      <c r="J10" s="64">
+      <c r="J10" s="47">
         <v>3.7975000000000002E-2</v>
       </c>
-      <c r="K10" s="61">
+      <c r="K10" s="46">
         <v>49</v>
       </c>
-      <c r="L10" s="61">
+      <c r="L10" s="46">
         <v>25</v>
       </c>
-      <c r="M10" s="61">
+      <c r="M10" s="46">
         <v>31</v>
       </c>
-      <c r="N10" s="68"/>
-      <c r="O10" s="61"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="46"/>
     </row>
     <row r="11" spans="1:16" ht="21">
-      <c r="A11" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="66"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="66"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="61">
+      <c r="A11" s="46" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="56"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="46">
         <v>3</v>
       </c>
-      <c r="G11" s="66"/>
-      <c r="H11" s="66"/>
-      <c r="I11" s="61">
+      <c r="G11" s="56"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="46">
         <v>10.199999999999999</v>
       </c>
-      <c r="J11" s="64">
+      <c r="J11" s="47">
         <v>3.7975000000000002E-2</v>
       </c>
-      <c r="K11" s="61">
+      <c r="K11" s="46">
         <v>49</v>
       </c>
-      <c r="L11" s="61">
+      <c r="L11" s="46">
         <v>25</v>
       </c>
-      <c r="M11" s="61">
+      <c r="M11" s="46">
         <v>31</v>
       </c>
-      <c r="N11" s="68"/>
-      <c r="O11" s="61"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="46"/>
     </row>
     <row r="12" spans="1:16" ht="21">
-      <c r="A12" s="61" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="70"/>
-      <c r="F12" s="61">
+      <c r="A12" s="46" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="57"/>
+      <c r="C12" s="57"/>
+      <c r="D12" s="57"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="46">
         <v>4</v>
       </c>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="61">
+      <c r="G12" s="57"/>
+      <c r="H12" s="57"/>
+      <c r="I12" s="46">
         <v>10.199999999999999</v>
       </c>
-      <c r="J12" s="64">
+      <c r="J12" s="47">
         <v>3.7975000000000002E-2</v>
       </c>
-      <c r="K12" s="61">
+      <c r="K12" s="46">
         <v>49</v>
       </c>
-      <c r="L12" s="61">
+      <c r="L12" s="46">
         <v>25</v>
       </c>
-      <c r="M12" s="61">
+      <c r="M12" s="46">
         <v>31</v>
       </c>
-      <c r="N12" s="71"/>
-      <c r="O12" s="61"/>
+      <c r="N12" s="60"/>
+      <c r="O12" s="46"/>
     </row>
     <row r="13" spans="1:16" ht="22.5">
-      <c r="A13" s="72"/>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="48"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="33">
         <v>4</v>
       </c>
@@ -1704,24 +1710,22 @@
       <c r="I13" s="33">
         <v>40.799999999999997</v>
       </c>
-      <c r="J13" s="73">
+      <c r="J13" s="49">
         <v>0.15190000000000001</v>
       </c>
       <c r="K13" s="33"/>
       <c r="L13" s="33"/>
       <c r="M13" s="33"/>
-      <c r="N13" s="74"/>
-      <c r="O13" s="75"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="H9:H12"/>
-    <mergeCell ref="N9:N12"/>
-    <mergeCell ref="B9:B12"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="D9:D12"/>
-    <mergeCell ref="E9:E12"/>
-    <mergeCell ref="G9:G12"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="N6:N7"/>
     <mergeCell ref="K2:M2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D5:D7"/>
@@ -1732,11 +1736,13 @@
     <mergeCell ref="K5:K7"/>
     <mergeCell ref="L5:L7"/>
     <mergeCell ref="M5:M7"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="E6:E7"/>
-    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="H9:H12"/>
+    <mergeCell ref="N9:N12"/>
+    <mergeCell ref="B9:B12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:D12"/>
+    <mergeCell ref="E9:E12"/>
+    <mergeCell ref="G9:G12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>